<commit_message>
new york products and new jersey products go to respective order forms when ordered
</commit_message>
<xml_diff>
--- a/order_forms/current_order.xlsx
+++ b/order_forms/current_order.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="162">
   <si>
-    <t>test</t>
+    <t>FIVE STAR SOUVENIRS INC..</t>
   </si>
   <si>
     <t>ORDER FORM</t>
@@ -4470,7 +4470,9 @@
       <c r="Q42" s="65">
         <v>1</v>
       </c>
-      <c r="R42" s="44"/>
+      <c r="R42" s="44">
+        <v>1</v>
+      </c>
       <c r="S42" s="65" t="s">
         <v>111</v>
       </c>
@@ -4519,7 +4521,9 @@
       <c r="Q43" s="154">
         <v>2</v>
       </c>
-      <c r="R43" s="136"/>
+      <c r="R43" s="136">
+        <v>4</v>
+      </c>
       <c r="S43" s="154" t="s">
         <v>115</v>
       </c>

</xml_diff>